<commit_message>
Openai cosine similarities update
</commit_message>
<xml_diff>
--- a/local_results.xlsx
+++ b/local_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehar\Documents\code-search-benchmarking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehar\Documents\Code-Search-Models\code-search-benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536217DA-0D21-4F0D-BBA0-AA7CC46DABEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA4CF18-5C29-44EC-90DA-A8E8310E7151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F0BE8C6-9BFF-4E76-96C1-AB035EF10842}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,26 +607,26 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <v>74.350999287107001</v>
+        <v>77.892614657367901</v>
       </c>
       <c r="C5" s="3">
-        <v>67.502302737460596</v>
+        <v>68.593206345652106</v>
       </c>
       <c r="D5" s="3">
-        <v>85.811284213145299</v>
+        <v>87.923206775194302</v>
       </c>
       <c r="E5" s="3">
-        <v>68.061019853671297</v>
+        <v>68.241956407044299</v>
       </c>
       <c r="F5" s="3">
-        <v>71.892902613535398</v>
+        <v>73.752703185625904</v>
       </c>
       <c r="G5" s="3">
-        <v>60.800736308881497</v>
+        <v>61.259439894891997</v>
       </c>
       <c r="H5" s="5">
         <f>AVERAGE(B5:G5)</f>
-        <v>71.403207502300177</v>
+        <v>72.943854544296087</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -634,32 +634,32 @@
         <v>22</v>
       </c>
       <c r="B6" s="3">
-        <f>AVERAGE(B3:B5)</f>
-        <v>74.966052064246256</v>
+        <f t="shared" ref="B6:H6" si="0">AVERAGE(B3:B5)</f>
+        <v>76.146590520999894</v>
       </c>
       <c r="C6" s="3">
-        <f>AVERAGE(C3:C5)</f>
-        <v>68.914262651242538</v>
+        <f t="shared" si="0"/>
+        <v>69.27789718730638</v>
       </c>
       <c r="D6" s="3">
-        <f>AVERAGE(D3:D5)</f>
-        <v>89.289576068270534</v>
+        <f t="shared" si="0"/>
+        <v>89.993550255620207</v>
       </c>
       <c r="E6" s="3">
-        <f>AVERAGE(E3:E5)</f>
-        <v>71.260432835026492</v>
+        <f t="shared" si="0"/>
+        <v>71.320745019484164</v>
       </c>
       <c r="F6" s="3">
-        <f>AVERAGE(F3:F5)</f>
-        <v>72.824753935742535</v>
+        <f t="shared" si="0"/>
+        <v>73.444687459772709</v>
       </c>
       <c r="G6" s="3">
-        <f>AVERAGE(G3:G5)</f>
-        <v>65.709782905990195</v>
+        <f t="shared" si="0"/>
+        <v>65.862684101327034</v>
       </c>
       <c r="H6" s="5">
-        <f>AVERAGE(H3:H5)</f>
-        <v>73.827476743419766</v>
+        <f t="shared" si="0"/>
+        <v>74.341025757418393</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -716,7 +716,7 @@
         <v>55.110880403893802</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" ref="H10:H18" si="0">AVERAGE(B10:G10)</f>
+        <f t="shared" ref="H10:H18" si="1">AVERAGE(B10:G10)</f>
         <v>64.099545745427264</v>
       </c>
     </row>
@@ -743,7 +743,7 @@
         <v>47.674977989789198</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61.236682582183164</v>
       </c>
     </row>
@@ -770,7 +770,7 @@
         <v>43.4723866566205</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60.099471496224169</v>
       </c>
     </row>
@@ -797,7 +797,7 @@
         <v>53.319525603633799</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.059254941532309</v>
       </c>
     </row>
@@ -824,7 +824,7 @@
         <v>46.170682684471103</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60.445763497419655</v>
       </c>
     </row>
@@ -851,7 +851,7 @@
         <v>43.4723866566205</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60.198280626927748</v>
       </c>
     </row>
@@ -878,7 +878,7 @@
         <v>40.876315214899698</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.834802930303304</v>
       </c>
     </row>
@@ -905,7 +905,7 @@
         <v>45.702698309812398</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60.993591231955996</v>
       </c>
     </row>
@@ -932,7 +932,7 @@
         <v>35.6469691715604</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49.526124728834027</v>
       </c>
     </row>
@@ -941,31 +941,31 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <f>AVERAGE(B10:B18)</f>
+        <f t="shared" ref="B19:H19" si="2">AVERAGE(B10:B18)</f>
         <v>63.16762409138174</v>
       </c>
       <c r="C19">
-        <f>AVERAGE(C10:C18)</f>
+        <f t="shared" si="2"/>
         <v>51.743722009077878</v>
       </c>
       <c r="D19">
-        <f>AVERAGE(D10:D18)</f>
+        <f t="shared" si="2"/>
         <v>81.90463349389745</v>
       </c>
       <c r="E19">
-        <f>AVERAGE(E10:E18)</f>
+        <f t="shared" si="2"/>
         <v>58.099803760696759</v>
       </c>
       <c r="F19">
-        <f>AVERAGE(F10:F18)</f>
+        <f t="shared" si="2"/>
         <v>55.696914866451088</v>
       </c>
       <c r="G19">
-        <f>AVERAGE(G10:G18)</f>
+        <f t="shared" si="2"/>
         <v>45.71631363236682</v>
       </c>
       <c r="H19" s="5">
-        <f>AVERAGE(H10:H18)</f>
+        <f t="shared" si="2"/>
         <v>59.388168642311953</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Test Result Updates
</commit_message>
<xml_diff>
--- a/local_results.xlsx
+++ b/local_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehar\Documents\Code-Search-Models\code-search-benchmarking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehar\Documents\code-search-benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA4CF18-5C29-44EC-90DA-A8E8310E7151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1998C36C-ED7D-405C-B4AD-F4C37DBF855F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F0BE8C6-9BFF-4E76-96C1-AB035EF10842}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,26 +607,26 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <v>77.892614657367901</v>
+        <v>74.294243934442804</v>
       </c>
       <c r="C5" s="3">
-        <v>68.593206345652106</v>
+        <v>67.508716647607301</v>
       </c>
       <c r="D5" s="3">
-        <v>87.923206775194302</v>
+        <v>85.731714618792694</v>
       </c>
       <c r="E5" s="3">
-        <v>68.241956407044299</v>
+        <v>68.029270579492305</v>
       </c>
       <c r="F5" s="3">
-        <v>73.752703185625904</v>
+        <v>71.938878273698506</v>
       </c>
       <c r="G5" s="3">
-        <v>61.259439894891997</v>
+        <v>60.822865220460301</v>
       </c>
       <c r="H5" s="5">
         <f>AVERAGE(B5:G5)</f>
-        <v>72.943854544296087</v>
+        <v>71.387614879082307</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -635,31 +635,31 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ref="B6:H6" si="0">AVERAGE(B3:B5)</f>
-        <v>76.146590520999894</v>
+        <v>74.94713361335819</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>69.27789718730638</v>
+        <v>68.91640062129143</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>89.993550255620207</v>
+        <v>89.263052870153004</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>71.320745019484164</v>
+        <v>71.249849743633504</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>73.444687459772709</v>
+        <v>72.8400791557969</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>65.862684101327034</v>
+        <v>65.717159209849797</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>74.341025757418393</v>
+        <v>73.822279202347147</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -752,26 +752,26 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>64.156029158456803</v>
+        <v>64.189865503518504</v>
       </c>
       <c r="C12" s="3">
-        <v>52.936056548612903</v>
+        <v>53.1955242383737</v>
       </c>
       <c r="D12" s="3">
-        <v>83.027475298063194</v>
+        <v>84.528207751115801</v>
       </c>
       <c r="E12" s="3">
-        <v>60.284503869258103</v>
+        <v>61.523248158503698</v>
       </c>
       <c r="F12" s="3">
-        <v>56.720377446333501</v>
+        <v>54.642694910491798</v>
       </c>
       <c r="G12" s="3">
-        <v>43.4723866566205</v>
+        <v>34.956792802720599</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="1"/>
-        <v>60.099471496224169</v>
+        <v>58.839388894120681</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -942,31 +942,31 @@
       </c>
       <c r="B19">
         <f t="shared" ref="B19:H19" si="2">AVERAGE(B10:B18)</f>
-        <v>63.16762409138174</v>
+        <v>63.171383685277483</v>
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>51.743722009077878</v>
+        <v>51.772551752384636</v>
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>81.90463349389745</v>
+        <v>82.07138154423663</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>58.099803760696759</v>
+        <v>58.237442015057383</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>55.696914866451088</v>
+        <v>55.466061251357566</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>45.71631363236682</v>
+        <v>44.770136537489051</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="2"/>
-        <v>59.388168642311953</v>
+        <v>59.248159464300457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>